<commit_message>
updated document sample excel files
</commit_message>
<xml_diff>
--- a/public/files/import/recurring-bills.xlsx
+++ b/public/files/import/recurring-bills.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13620" firstSheet="3" activeTab="5"/>
+    <workbookView windowWidth="28800" windowHeight="13660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="recurring" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>recurable_type</t>
   </si>
@@ -123,6 +123,18 @@
     <t>notes</t>
   </si>
   <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>subheading</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
     <t>draft</t>
   </si>
   <si>
@@ -141,6 +153,15 @@
     <t>can@gmail.com</t>
   </si>
   <si>
+    <t>bill</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>#55588b</t>
+  </si>
+  <si>
     <t>item_name</t>
   </si>
   <si>
@@ -166,6 +187,9 @@
   </si>
   <si>
     <t>product</t>
+  </si>
+  <si>
+    <t>tax_name</t>
   </si>
   <si>
     <t>tax_rate</t>
@@ -209,13 +233,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -231,6 +255,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF98C379"/>
+      <name val="Menlo"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -260,6 +290,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -276,18 +329,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -299,6 +359,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,73 +403,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -389,12 +419,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -407,13 +503,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,145 +545,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,6 +604,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -586,11 +655,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,181 +704,127 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -803,30 +833,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1262,10 +1295,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
@@ -1288,7 +1321,7 @@
     <col min="21" max="21" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1352,13 +1385,25 @@
       <c r="U1" t="s">
         <v>33</v>
       </c>
+      <c r="V1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1">
         <v>45152</v>
@@ -1370,25 +1415,34 @@
         <v>900</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H2" s="2">
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="V2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1426,25 +1480,25 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1452,10 +1506,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1480,31 +1534,34 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.5625" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="2" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5625" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1539,10 +1596,10 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1550,13 +1607,13 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1571,7 +1628,7 @@
   <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1589,16 +1646,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1606,10 +1663,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D2">
         <v>1000</v>
@@ -1623,10 +1680,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D3">
         <v>100</v>
@@ -1640,10 +1697,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D4">
         <v>900</v>

</xml_diff>